<commit_message>
Napravljena prva verzija zaključka u dokumentaciji.
</commit_message>
<xml_diff>
--- a/funkcionalnosti.xlsx
+++ b/funkcionalnosti.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\Semestar5\progi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\Semestar5\progi\SourceresOfTheNorth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98979BE7-97FC-4A83-8EF0-FDC1CEF491E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0309D9B6-C452-4550-95B7-CB3302D0AA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22519CCB-3667-43AA-AF5C-DE329FEBDB8B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Funkcionalnost</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>čitanje lokacije iz metapodataka slike</t>
+  </si>
+  <si>
+    <t>dvojezičnost</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -192,65 +195,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -281,52 +225,172 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98987AE6-BAB1-4B64-94F0-88C88426CBDB}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,273 +721,282 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="14"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="14"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="14"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="14"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="14"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="2"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="8"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dokumentirano ispitivanje komponenti, u upitama za puštanje u pogon dodan popis inicijalnih podataka spremljenih u bazi podataka, još neki mali popravci.
</commit_message>
<xml_diff>
--- a/funkcionalnosti.xlsx
+++ b/funkcionalnosti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\Semestar5\progi\SourceresOfTheNorth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0309D9B6-C452-4550-95B7-CB3302D0AA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0AABD-4D58-403B-93EB-48DAB05AD16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22519CCB-3667-43AA-AF5C-DE329FEBDB8B}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{22519CCB-3667-43AA-AF5C-DE329FEBDB8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,10 +144,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -351,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,6 +398,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,9 +428,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -449,7 +468,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -555,7 +574,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -697,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98987AE6-BAB1-4B64-94F0-88C88426CBDB}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,26 +805,26 @@
       <c r="A7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3"/>
     </row>
@@ -813,8 +832,8 @@
       <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3"/>
     </row>
@@ -831,8 +850,8 @@
       <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
     </row>
@@ -840,8 +859,8 @@
       <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3"/>
     </row>
@@ -876,8 +895,8 @@
       <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="4"/>
       <c r="E17" s="3"/>
     </row>
@@ -894,7 +913,6 @@
       <c r="A19" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3"/>
@@ -903,8 +921,8 @@
       <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>
     </row>
@@ -912,8 +930,8 @@
       <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
     </row>
@@ -921,8 +939,8 @@
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="4"/>
       <c r="E22" s="3"/>
     </row>
@@ -930,8 +948,8 @@
       <c r="A23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
     </row>
@@ -939,8 +957,8 @@
       <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3"/>
     </row>
@@ -948,8 +966,8 @@
       <c r="A25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
     </row>
@@ -958,7 +976,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="14"/>
-      <c r="C26" s="4"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
     </row>
@@ -966,9 +984,9 @@
       <c r="A27" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="14"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -985,7 +1003,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="14"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="4"/>
       <c r="E29" s="3"/>
     </row>
@@ -998,6 +1016,9 @@
       <c r="D30" s="4"/>
       <c r="E30" s="3"/>
     </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Popravak opisa baze podataka i dijagrama aktivnosti, male korekcije po cijeloj dokumentaciji.
</commit_message>
<xml_diff>
--- a/funkcionalnosti.xlsx
+++ b/funkcionalnosti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faks\Semestar5\progi\SourceresOfTheNorth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0AABD-4D58-403B-93EB-48DAB05AD16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828E1A79-5702-4F67-8C2E-1284D29E2BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{22519CCB-3667-43AA-AF5C-DE329FEBDB8B}"/>
   </bookViews>
@@ -401,13 +401,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98987AE6-BAB1-4B64-94F0-88C88426CBDB}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,8 +796,8 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
@@ -807,107 +805,107 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -921,7 +919,7 @@
       <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="7"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>
@@ -930,7 +928,7 @@
       <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="7"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
@@ -939,7 +937,7 @@
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="22"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="7"/>
       <c r="D22" s="4"/>
       <c r="E22" s="3"/>
@@ -948,7 +946,7 @@
       <c r="A23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="7"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
@@ -957,7 +955,7 @@
       <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="7"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3"/>
@@ -966,7 +964,7 @@
       <c r="A25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="22"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="7"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
@@ -976,7 +974,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="14"/>
-      <c r="C26" s="19"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
     </row>
@@ -1016,9 +1014,6 @@
       <c r="D30" s="4"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="21"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>